<commit_message>
setup and test i18n, added TODO LIST to Readme as reminder
</commit_message>
<xml_diff>
--- a/lib/data_imports/data_collected.xlsx
+++ b/lib/data_imports/data_collected.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/shop_titan_tool_web/lib/data_imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9435BC42-4910-E346-8FF5-CCAB4C77ACE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD89E005-F51E-7742-982B-0C9EE6AB7759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="1260" windowWidth="28300" windowHeight="16960" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="2" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
+    <sheet name="MonthlyEvents" sheetId="2" r:id="rId2"/>
+    <sheet name="OneTimeEvents" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -223,6 +225,258 @@
   </si>
   <si>
     <t>treasures/keys</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duration</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reccurence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon_url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lost_city_of_gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dragon_invasion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kings_caprice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tower_of_titans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5 days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7 days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4 days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>28 days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/lost_city_of_gold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/dragon_invasion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/kings_caprice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/tower_of_titans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_en</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_zh</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Full Bloom Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Christmas Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vampire Masquerade Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bjron Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spacefarer Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year of the Rabbit Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Halloween Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>christmas_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>full_bloom_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_of_dragon_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vampire_masquerade_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bjorn_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spacefarer_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_of_the_rabbit_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>year_of_the_tiger_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year of the Tiger Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avatar Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>avatar_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>降世神通：最后的气宗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>春暖花开内容令状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圣诞内容令状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小淘气内容令状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比约恩内容令状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>遨游太空内容令状</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>兔年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022年万圣节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>虎年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2022年五月五日节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cinco_de_mayo_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cinco de Mayo Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>halloween2022_pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Year of the Dragon Content Pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/full_bloom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/year_of_dragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/christmas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/vampire</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/bjorn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/spacefarer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/year_of_rabbit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/halloween2022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/year_of_tiger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/avatar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>events/content_pass/cinco_de_mayo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -269,8 +523,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -609,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D01BB35-1EFF-8142-8049-CC58E4897854}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -879,4 +1136,373 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CE4324-2568-3749-AED0-5A678396A05D}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43791</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44742</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44083</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44008</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA03D614-9D25-014E-BEA0-F56DD3E0919C}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="1">
+        <v>45370</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45385</v>
+      </c>
+      <c r="F2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45314</v>
+      </c>
+      <c r="E3" s="1">
+        <v>45341</v>
+      </c>
+      <c r="F3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45282</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45299</v>
+      </c>
+      <c r="F4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45202</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45230</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45146</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45161</v>
+      </c>
+      <c r="F6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45062</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45089</v>
+      </c>
+      <c r="F7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44936</v>
+      </c>
+      <c r="E8" s="1">
+        <v>44965</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44859</v>
+      </c>
+      <c r="E9" s="1">
+        <v>44866</v>
+      </c>
+      <c r="F9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44585</v>
+      </c>
+      <c r="E10" s="1">
+        <v>44598</v>
+      </c>
+      <c r="F10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44501</v>
+      </c>
+      <c r="E11" s="1">
+        <v>44530</v>
+      </c>
+      <c r="F11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44683</v>
+      </c>
+      <c r="E12" s="1">
+        <v>44710</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished tasks for importing monthly events and content pass
</commit_message>
<xml_diff>
--- a/lib/data_imports/data_collected.xlsx
+++ b/lib/data_imports/data_collected.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/shop_titan_tool_web/lib/data_imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD89E005-F51E-7742-982B-0C9EE6AB7759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D271596-5284-2D47-84DC-8CFA50D32231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="2" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
     <sheet name="MonthlyEvents" sheetId="2" r:id="rId2"/>
-    <sheet name="OneTimeEvents" sheetId="3" r:id="rId3"/>
+    <sheet name="ContentPass" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1249,256 +1249,257 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
-    <col min="2" max="2" width="32.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.83203125" customWidth="1"/>
+    <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>65</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1">
+        <v>45370</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45385</v>
+      </c>
+      <c r="D2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" t="s">
         <v>66</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>85</v>
-      </c>
-      <c r="D2" s="1">
-        <v>45370</v>
-      </c>
-      <c r="E2" s="1">
-        <v>45385</v>
-      </c>
-      <c r="F2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>75</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1">
+        <v>45314</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45341</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
         <v>98</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>86</v>
-      </c>
-      <c r="D3" s="1">
-        <v>45314</v>
-      </c>
-      <c r="E3" s="1">
-        <v>45341</v>
-      </c>
-      <c r="F3" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>73</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1">
+        <v>45282</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45299</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
         <v>67</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>87</v>
-      </c>
-      <c r="D4" s="1">
-        <v>45282</v>
-      </c>
-      <c r="E4" s="1">
-        <v>45299</v>
-      </c>
-      <c r="F4" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>76</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1">
+        <v>45202</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45230</v>
+      </c>
+      <c r="D5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>88</v>
-      </c>
-      <c r="D5" s="1">
-        <v>45202</v>
-      </c>
-      <c r="E5" s="1">
-        <v>45230</v>
-      </c>
-      <c r="F5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>77</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1">
+        <v>45146</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45161</v>
+      </c>
+      <c r="D6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E6" t="s">
         <v>69</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>89</v>
-      </c>
-      <c r="D6" s="1">
-        <v>45146</v>
-      </c>
-      <c r="E6" s="1">
-        <v>45161</v>
-      </c>
-      <c r="F6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>78</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1">
+        <v>45062</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45089</v>
+      </c>
+      <c r="D7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" t="s">
         <v>70</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" t="s">
         <v>90</v>
-      </c>
-      <c r="D7" s="1">
-        <v>45062</v>
-      </c>
-      <c r="E7" s="1">
-        <v>45089</v>
-      </c>
-      <c r="F7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>79</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1">
+        <v>44936</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44965</v>
+      </c>
+      <c r="D8" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" t="s">
         <v>71</v>
       </c>
-      <c r="C8" t="s">
+      <c r="F8" t="s">
         <v>91</v>
-      </c>
-      <c r="D8" s="1">
-        <v>44936</v>
-      </c>
-      <c r="E8" s="1">
-        <v>44965</v>
-      </c>
-      <c r="F8" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>97</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1">
+        <v>44859</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44866</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E9" t="s">
         <v>72</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>92</v>
-      </c>
-      <c r="D9" s="1">
-        <v>44859</v>
-      </c>
-      <c r="E9" s="1">
-        <v>44866</v>
-      </c>
-      <c r="F9" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>80</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1">
+        <v>44585</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44598</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
         <v>81</v>
       </c>
-      <c r="C10" t="s">
+      <c r="F10" t="s">
         <v>93</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44585</v>
-      </c>
-      <c r="E10" s="1">
-        <v>44598</v>
-      </c>
-      <c r="F10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>83</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1">
+        <v>44501</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44530</v>
+      </c>
+      <c r="D11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" t="s">
         <v>82</v>
       </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>84</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44501</v>
-      </c>
-      <c r="E11" s="1">
-        <v>44530</v>
-      </c>
-      <c r="F11" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>95</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1">
+        <v>44683</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44710</v>
+      </c>
+      <c r="D12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" t="s">
         <v>96</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>94</v>
-      </c>
-      <c r="D12" s="1">
-        <v>44683</v>
-      </c>
-      <c r="E12" s="1">
-        <v>44710</v>
-      </c>
-      <c r="F12" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug-fix: calendar month translation
</commit_message>
<xml_diff>
--- a/lib/data_imports/data_collected.xlsx
+++ b/lib/data_imports/data_collected.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/shop_titan_tool_web/lib/data_imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D271596-5284-2D47-84DC-8CFA50D32231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE6B14D-C1F4-6E41-9345-4544680B4873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="2" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="3" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
     <sheet name="MonthlyEvents" sheetId="2" r:id="rId2"/>
     <sheet name="ContentPass" sheetId="3" r:id="rId3"/>
+    <sheet name="Booster" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -477,6 +478,26 @@
   </si>
   <si>
     <t>events/content_pass/cinco_de_mayo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Category</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>top_quality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>booster</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 day</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>end_time/recur</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -484,7 +505,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -499,6 +520,18 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF569CD6"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -523,11 +556,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1248,7 +1290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA03D614-9D25-014E-BEA0-F56DD3E0919C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1506,4 +1548,109 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196C4610-BC82-6741-A3D8-2966B31C8394}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45391</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="I3" s="4"/>
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="I4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="I5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="I6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="I7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="I8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="I9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="I10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="I11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="I12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="I13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adjust lost city of gold event time, calendar css finished
</commit_message>
<xml_diff>
--- a/lib/data_imports/data_collected.xlsx
+++ b/lib/data_imports/data_collected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/shop_titan_tool_web/lib/data_imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE6B14D-C1F4-6E41-9345-4544680B4873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AC05DB-3D58-FB42-954E-ECE44055086B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="3" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="1" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -1184,8 +1184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CE4324-2568-3749-AED0-5A678396A05D}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1217,7 +1217,7 @@
         <v>51</v>
       </c>
       <c r="B2" s="1">
-        <v>43791</v>
+        <v>44022</v>
       </c>
       <c r="C2" t="s">
         <v>57</v>
@@ -1554,7 +1554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196C4610-BC82-6741-A3D8-2966B31C8394}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add a sort-by tab in filter container, contents not implemented yet
</commit_message>
<xml_diff>
--- a/lib/data_imports/data_collected.xlsx
+++ b/lib/data_imports/data_collected.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/shop_titan_tool_web/lib/data_imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AC05DB-3D58-FB42-954E-ECE44055086B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823DE2BB-C61F-274D-90A3-396C69DFB68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="1" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="3" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="120">
   <si>
     <t>unlock_merchant_level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -489,15 +489,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>booster</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1 day</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>end_time/recur</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hero_merchant_xp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>crafting_quality</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>surcharge_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>better_deals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -556,7 +576,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -570,6 +590,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1184,7 +1207,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CE4324-2568-3749-AED0-5A678396A05D}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1552,21 +1575,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196C4610-BC82-6741-A3D8-2966B31C8394}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="2" max="3" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1574,79 +1597,115 @@
         <v>110</v>
       </c>
       <c r="C1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
-        <v>114</v>
-      </c>
       <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="J1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>111</v>
       </c>
       <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45391</v>
+      </c>
+      <c r="E2" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="2">
-        <v>45391</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="I3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="I4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="I5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="I6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="I7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="I8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="I9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="I10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="I11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="I12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="I13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45393</v>
+      </c>
+      <c r="E3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45398</v>
+      </c>
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="J6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="J7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="J8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="J9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="J10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="J11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="J12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="J13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update kings caprice date, fixed weekday translation
</commit_message>
<xml_diff>
--- a/lib/data_imports/data_collected.xlsx
+++ b/lib/data_imports/data_collected.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhimoye/environment/shop_titan_tool_web/lib/data_imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823DE2BB-C61F-274D-90A3-396C69DFB68C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82FC900-67DD-864D-B3F7-F6F53F0E7888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="3" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
+    <workbookView xWindow="720" yWindow="1500" windowWidth="28300" windowHeight="14900" activeTab="1" xr2:uid="{12806AD4-EDD1-E74D-A0E6-8A783616F34F}"/>
   </bookViews>
   <sheets>
     <sheet name="FlashQuests" sheetId="1" r:id="rId1"/>
@@ -1207,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CE4324-2568-3749-AED0-5A678396A05D}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1274,7 +1274,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="1">
-        <v>44083</v>
+        <v>44756</v>
       </c>
       <c r="C4" t="s">
         <v>56</v>
@@ -1577,7 +1577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{196C4610-BC82-6741-A3D8-2966B31C8394}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>